<commit_message>
update name to main
</commit_message>
<xml_diff>
--- a/Amor_librorum.xlsx
+++ b/Amor_librorum.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inholland-my.sharepoint.com/personal/frank_brandse_inholland_nl/Documents/H-schijf/FrankB/ProjectDatabases/2122/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inholland-my.sharepoint.com/personal/682062_student_inholland_nl/Documents/Inholland/ME1_4/AmorLibrorum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="276" documentId="11_F25DC773A252ABDACC104853D91F7F0E5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E2B773F-5019-4D44-8BF7-C209C360B59D}"/>
+  <xr:revisionPtr revIDLastSave="277" documentId="11_F25DC773A252ABDACC104853D91F7F0E5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05F6CE3C-9FE3-8449-BCA8-FE453467CFB6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="books" sheetId="1" r:id="rId1"/>
@@ -34,8 +34,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="90">
   <si>
     <t>title</t>
   </si>
@@ -636,26 +658,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" customWidth="1"/>
-    <col min="2" max="2" width="23.6328125" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" customWidth="1"/>
-    <col min="4" max="4" width="16.36328125" customWidth="1"/>
-    <col min="5" max="5" width="17.90625" customWidth="1"/>
-    <col min="6" max="6" width="18.08984375" customWidth="1"/>
-    <col min="7" max="7" width="13.6328125" customWidth="1"/>
-    <col min="8" max="8" width="12.1796875" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="25.36328125" customWidth="1"/>
+    <col min="10" max="10" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -687,7 +709,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -710,7 +732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -734,7 +756,7 @@
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -757,7 +779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -783,7 +805,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -806,7 +828,7 @@
         <v>42867</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -829,7 +851,7 @@
         <v>43154</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>80</v>
       </c>
@@ -855,7 +877,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -881,7 +903,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -907,7 +929,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>77</v>
       </c>
@@ -930,7 +952,7 @@
         <v>44147</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -953,7 +975,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -976,7 +998,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -1002,7 +1024,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1025,7 +1047,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1051,7 +1073,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1074,7 +1096,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1100,7 +1122,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -1123,7 +1145,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -1140,7 +1162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -1163,7 +1185,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>83</v>
       </c>
@@ -1189,7 +1211,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>86</v>
       </c>
@@ -1215,7 +1237,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -1231,11 +1253,12 @@
       <c r="I24">
         <v>2</v>
       </c>
-      <c r="J24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J24" t="e" cm="1">
+        <f t="array" ref="J24">French</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -1258,7 +1281,7 @@
         <v>41076</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -1284,7 +1307,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -1307,7 +1330,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -1333,7 +1356,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -1356,7 +1379,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>73</v>
       </c>
@@ -1379,7 +1402,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>76</v>
       </c>

</xml_diff>